<commit_message>
Updated field for basic L3 interfaces and SNMP variables amongst others. Updated sample spreadsheet.
</commit_message>
<xml_diff>
--- a/inventory.xlsx
+++ b/inventory.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27106"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27610"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paul/Documents/ansible/sw-config-dynamic/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/paulowen/Documents/git/sw-config-dynamic/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -32,19 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="49">
-  <si>
-    <t>SW1</t>
-  </si>
-  <si>
-    <t>VLAN10</t>
-  </si>
-  <si>
-    <t>VLAN20</t>
-  </si>
-  <si>
-    <t>VLAN30</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="51">
   <si>
     <t>Switchport Type</t>
   </si>
@@ -67,54 +55,6 @@
     <t>True/False</t>
   </si>
   <si>
-    <t>GigabitEthernet1/0/2</t>
-  </si>
-  <si>
-    <t>TEST_ACCESS</t>
-  </si>
-  <si>
-    <t>TEST_TRUNK</t>
-  </si>
-  <si>
-    <t>1-999</t>
-  </si>
-  <si>
-    <t>sw1user</t>
-  </si>
-  <si>
-    <t>yeahrightomate</t>
-  </si>
-  <si>
-    <t>GigabitEthernet1/0/3</t>
-  </si>
-  <si>
-    <t>SW2</t>
-  </si>
-  <si>
-    <t>VLAN40</t>
-  </si>
-  <si>
-    <t>VLAN50</t>
-  </si>
-  <si>
-    <t>VLAN60</t>
-  </si>
-  <si>
-    <t>sw2user</t>
-  </si>
-  <si>
-    <t>cooldude</t>
-  </si>
-  <si>
-    <t>TEST_ACCESS2</t>
-  </si>
-  <si>
-    <t>TEST_ACCESS3</t>
-  </si>
-  <si>
-    <t>corp.local</t>
-  </si>
-  <si>
     <t>Device</t>
   </si>
   <si>
@@ -151,34 +91,100 @@
     <t>Native VLAN</t>
   </si>
   <si>
-    <t>TEST_ROUTED</t>
-  </si>
-  <si>
-    <t>range GigabitEthernet1/0/3 - 20</t>
-  </si>
-  <si>
-    <t>DATA</t>
-  </si>
-  <si>
-    <t>YELO</t>
-  </si>
-  <si>
-    <t>SW3</t>
-  </si>
-  <si>
-    <t>paul</t>
-  </si>
-  <si>
-    <t>bang!</t>
-  </si>
-  <si>
-    <t>home.local</t>
-  </si>
-  <si>
-    <t>WORD</t>
-  </si>
-  <si>
-    <t>range GigabitEthernet1/0/1 - 48</t>
+    <t>GigabitEthernet2/0/1</t>
+  </si>
+  <si>
+    <t>IP Address</t>
+  </si>
+  <si>
+    <t>Gateway</t>
+  </si>
+  <si>
+    <t>range GigabitEthernet1/0/44 - 48</t>
+  </si>
+  <si>
+    <t>range GigabitEthernet2/0/2 - 48</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GigabitEthernet1/0/1 </t>
+  </si>
+  <si>
+    <t>SNMP Location</t>
+  </si>
+  <si>
+    <t>SNMPv2 RO Community</t>
+  </si>
+  <si>
+    <t>L3 Interfaces</t>
+  </si>
+  <si>
+    <t>L3 Description</t>
+  </si>
+  <si>
+    <t>range GigabitEthernet1/0/2 - 43</t>
+  </si>
+  <si>
+    <t>SWITCH1</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>domain.internal</t>
+  </si>
+  <si>
+    <t>STAFF</t>
+  </si>
+  <si>
+    <t>WIRELESS</t>
+  </si>
+  <si>
+    <t>MGMT</t>
+  </si>
+  <si>
+    <t>UPLINK</t>
+  </si>
+  <si>
+    <t>range GigabitEthernet1/0/2 - 48</t>
+  </si>
+  <si>
+    <t>10.1.1.1</t>
+  </si>
+  <si>
+    <t>Vlan100</t>
+  </si>
+  <si>
+    <t>Right Over There</t>
+  </si>
+  <si>
+    <t>public</t>
+  </si>
+  <si>
+    <t>SWITCH2</t>
+  </si>
+  <si>
+    <t>10.1.1.11/24</t>
+  </si>
+  <si>
+    <t>Right Over Here</t>
+  </si>
+  <si>
+    <t>SWITCH3</t>
+  </si>
+  <si>
+    <t>range GigabitEthernet1/0/2 - 24</t>
+  </si>
+  <si>
+    <t>10.1.1.12/24</t>
+  </si>
+  <si>
+    <t>10.1.1.13/24</t>
+  </si>
+  <si>
+    <t>Somewhere Nowhere</t>
   </si>
 </sst>
 </file>
@@ -241,8 +247,218 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="225">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -262,7 +478,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="225">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -270,6 +486,111 @@
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="200" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="202" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="204" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="206" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="208" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="210" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="212" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="214" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="216" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="218" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="220" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="222" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="224" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -277,6 +598,111 @@
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="189" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="191" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="193" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="195" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="197" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="199" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="201" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="203" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="205" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="207" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="209" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="211" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="213" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="215" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="217" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="219" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="221" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="223" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -552,284 +978,372 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M10"/>
+  <dimension ref="A1:S10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.1640625" customWidth="1"/>
-    <col min="5" max="5" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="41.83203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="5.6640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.83203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.83203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="47.5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="21.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>30</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="B2" t="s">
         <v>31</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="C2" t="s">
         <v>32</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="D2" t="s">
         <v>33</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" t="s">
-        <v>16</v>
-      </c>
-      <c r="D2" t="s">
-        <v>26</v>
       </c>
       <c r="E2">
         <v>10</v>
       </c>
       <c r="F2" t="s">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="G2" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="H2" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I2" t="s">
-        <v>12</v>
-      </c>
-      <c r="J2">
-        <v>10</v>
+        <v>37</v>
       </c>
       <c r="K2" t="b">
         <v>0</v>
       </c>
+      <c r="M2">
+        <v>100</v>
+      </c>
+      <c r="N2" t="s">
+        <v>39</v>
+      </c>
+      <c r="O2" t="s">
+        <v>40</v>
+      </c>
+      <c r="P2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>44</v>
+      </c>
+      <c r="R2" t="s">
+        <v>41</v>
+      </c>
+      <c r="S2" t="s">
+        <v>42</v>
+      </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="E3">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="F3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H3" t="s">
+        <v>1</v>
+      </c>
+      <c r="I3" t="s">
+        <v>34</v>
+      </c>
+      <c r="J3">
+        <v>10</v>
+      </c>
+      <c r="K3" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="E4">
+        <v>100</v>
+      </c>
+      <c r="F4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" t="s">
         <v>2</v>
       </c>
-      <c r="G3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" t="s">
-        <v>6</v>
-      </c>
-      <c r="I3" t="s">
-        <v>13</v>
-      </c>
-      <c r="K3" t="b">
+      <c r="I4" t="s">
+        <v>37</v>
+      </c>
+      <c r="K4" t="b">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="G5" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" t="s">
         <v>1</v>
       </c>
-      <c r="L3" t="s">
-        <v>14</v>
-      </c>
-      <c r="M3">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="E4">
-        <v>30</v>
-      </c>
-      <c r="F4" t="s">
-        <v>3</v>
-      </c>
-      <c r="G4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="G5" t="s">
-        <v>40</v>
-      </c>
-      <c r="H5" t="s">
-        <v>5</v>
-      </c>
       <c r="I5" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="J5">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="K5" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>43</v>
       </c>
       <c r="B6" t="s">
-        <v>22</v>
+        <v>31</v>
       </c>
       <c r="C6" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="D6" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="E6">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="F6" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="G6" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="H6" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="I6" t="s">
-        <v>12</v>
-      </c>
-      <c r="J6">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="K6" t="b">
         <v>0</v>
       </c>
+      <c r="M6">
+        <v>100</v>
+      </c>
+      <c r="N6" t="s">
+        <v>39</v>
+      </c>
+      <c r="O6" t="s">
+        <v>40</v>
+      </c>
+      <c r="P6" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>48</v>
+      </c>
+      <c r="R6" t="s">
+        <v>45</v>
+      </c>
+      <c r="S6" t="s">
+        <v>42</v>
+      </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.2">
       <c r="E7">
-        <v>50</v>
+        <v>11</v>
       </c>
       <c r="F7" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="G7" t="s">
+        <v>29</v>
+      </c>
+      <c r="H7" t="s">
+        <v>1</v>
+      </c>
+      <c r="I7" t="s">
+        <v>34</v>
+      </c>
+      <c r="J7">
+        <v>10</v>
+      </c>
+      <c r="K7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="E8">
+        <v>100</v>
+      </c>
+      <c r="F8" t="s">
+        <v>36</v>
+      </c>
+      <c r="G8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H8" t="s">
+        <v>2</v>
+      </c>
+      <c r="I8" t="s">
+        <v>35</v>
+      </c>
+      <c r="J8">
         <v>11</v>
-      </c>
-      <c r="H7" t="s">
-        <v>5</v>
-      </c>
-      <c r="I7" t="s">
-        <v>24</v>
-      </c>
-      <c r="J7">
-        <v>50</v>
-      </c>
-      <c r="K7" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="E8">
-        <v>60</v>
-      </c>
-      <c r="F8" t="s">
-        <v>21</v>
-      </c>
-      <c r="G8" t="s">
-        <v>17</v>
-      </c>
-      <c r="H8" t="s">
-        <v>5</v>
-      </c>
-      <c r="I8" t="s">
-        <v>25</v>
-      </c>
-      <c r="J8">
-        <v>60</v>
       </c>
       <c r="K8" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" t="s">
+        <v>31</v>
+      </c>
+      <c r="C9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" t="s">
+        <v>33</v>
+      </c>
       <c r="E9">
-        <v>70</v>
+        <v>10</v>
       </c>
       <c r="F9" t="s">
+        <v>34</v>
+      </c>
+      <c r="G9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H9" t="s">
+        <v>2</v>
+      </c>
+      <c r="I9" t="s">
+        <v>37</v>
+      </c>
+      <c r="K9" t="b">
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>100</v>
+      </c>
+      <c r="N9" t="s">
+        <v>39</v>
+      </c>
+      <c r="O9" t="s">
+        <v>40</v>
+      </c>
+      <c r="P9" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>49</v>
+      </c>
+      <c r="R9" t="s">
+        <v>50</v>
+      </c>
+      <c r="S9" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>43</v>
-      </c>
-      <c r="B10" t="s">
-        <v>44</v>
-      </c>
-      <c r="C10" t="s">
-        <v>45</v>
-      </c>
-      <c r="D10" t="s">
-        <v>46</v>
-      </c>
-      <c r="E10">
-        <v>999</v>
-      </c>
-      <c r="F10" t="s">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="G10" t="s">
         <v>47</v>
       </c>
-      <c r="G10" t="s">
-        <v>48</v>
-      </c>
       <c r="H10" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I10" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="J10">
-        <v>999</v>
+        <v>10</v>
       </c>
       <c r="K10" t="b">
         <v>0</v>
@@ -837,10 +1351,10 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H10">
       <formula1>Mode</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K3 K5:K8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K10">
       <formula1>TRUEFALSE</formula1>
     </dataValidation>
   </dataValidations>
@@ -864,15 +1378,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B2" t="b">
         <v>1</v>
@@ -880,7 +1394,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B3" t="b">
         <v>0</v>
@@ -888,7 +1402,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>